<commit_message>
Add code 99 to typeOfWeasponForceInvolved.
</commit_message>
<xml_diff>
--- a/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="20480" windowHeight="12320" tabRatio="705" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="20480" windowHeight="12320" tabRatio="705" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="663">
   <si>
     <t>Table</t>
   </si>
@@ -5194,7 +5194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
@@ -9491,10 +9491,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9678,25 +9678,36 @@
         <v>271</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1">
-      <c r="A17">
-        <v>99999</v>
-      </c>
-      <c r="B17" s="2">
-        <v>95</v>
-      </c>
-      <c r="C17" t="s">
-        <v>272</v>
+    <row r="17" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A17" s="1">
+        <v>999</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18">
+        <v>99999</v>
+      </c>
+      <c r="B18" s="2">
+        <v>95</v>
+      </c>
+      <c r="C18" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1">
+      <c r="A19">
         <v>99998</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>650</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the code table spreadsheets to be consistent with the spec.
Also update the load data table sql scripts.
</commit_message>
<xml_diff>
--- a/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="20480" windowHeight="12320" tabRatio="705" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="7780" yWindow="1080" windowWidth="20240" windowHeight="12160" tabRatio="705" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="676">
   <si>
     <t>Table</t>
   </si>
@@ -2038,13 +2038,52 @@
   </si>
   <si>
     <t>Replace</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>Cyberspace</t>
+  </si>
+  <si>
+    <t>Simple/Gross Neglect</t>
+  </si>
+  <si>
+    <t>Organized Abuse</t>
+  </si>
+  <si>
+    <t>Intentional Abuse and Torture</t>
+  </si>
+  <si>
+    <t>Animal Sexual Abuse (Bestiality)</t>
+  </si>
+  <si>
+    <t>Anti-Mormon</t>
+  </si>
+  <si>
+    <t>Anti-Jehovah’s Witness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti-Eastern Orthodox </t>
+  </si>
+  <si>
+    <t>Anti-Other Christian</t>
+  </si>
+  <si>
+    <t>Anti-Buddhist</t>
+  </si>
+  <si>
+    <t>Anti-Hindu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti-Sikh </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2074,6 +2113,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRomanPSMT"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2092,7 +2136,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2125,8 +2169,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2137,8 +2201,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="32">
+  <cellStyles count="52">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2154,6 +2222,16 @@
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2169,6 +2247,16 @@
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
@@ -2745,10 +2833,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2953,85 +3041,85 @@
         <v>533</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1">
+    <row r="15" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="1">
-        <v>32</v>
-      </c>
-      <c r="B15">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>287</v>
-      </c>
-      <c r="D15" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1">
+        <v>28</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="1">
-        <v>33</v>
-      </c>
-      <c r="B16">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>288</v>
+        <v>29</v>
+      </c>
+      <c r="B16" s="1">
+        <v>29</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>670</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="1">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B17">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D17" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="1">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B18">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="1">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>291</v>
-      </c>
-      <c r="D19" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D19" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="1">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>535</v>
@@ -3039,13 +3127,13 @@
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>535</v>
@@ -3053,83 +3141,83 @@
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1">
       <c r="A22" s="1">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B22">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>294</v>
-      </c>
-      <c r="D22" t="s">
-        <v>536</v>
+        <v>292</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1">
       <c r="A23" s="1">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B23">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
       <c r="A24" s="1">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B24">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D24" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1">
       <c r="A25" s="1">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B25">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1">
       <c r="A26" s="1">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B26">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>298</v>
-      </c>
-      <c r="D26" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D26" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1">
       <c r="A27" s="1">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B27">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>537</v>
@@ -3137,43 +3225,141 @@
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1">
       <c r="A28" s="1">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B28">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>300</v>
-      </c>
-      <c r="D28" t="s">
-        <v>273</v>
+        <v>298</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1">
       <c r="A29" s="1">
+        <v>72</v>
+      </c>
+      <c r="B29">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>299</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A30" s="1">
+        <v>81</v>
+      </c>
+      <c r="B30" s="1">
+        <v>81</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>671</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A31" s="1">
+        <v>82</v>
+      </c>
+      <c r="B31" s="1">
+        <v>82</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>672</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A32" s="1">
+        <v>83</v>
+      </c>
+      <c r="B32" s="1">
+        <v>83</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A33" s="1">
+        <v>84</v>
+      </c>
+      <c r="B33" s="1">
+        <v>84</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>674</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" s="1">
+        <v>85</v>
+      </c>
+      <c r="B34" s="1">
+        <v>85</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1">
+      <c r="A35" s="1">
+        <v>88</v>
+      </c>
+      <c r="B35">
+        <v>88</v>
+      </c>
+      <c r="C35" t="s">
+        <v>300</v>
+      </c>
+      <c r="D35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1">
+      <c r="A36" s="1">
         <v>99999</v>
       </c>
-      <c r="B29">
+      <c r="B36">
         <v>99</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C36" t="s">
         <v>301</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D36" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
+    <row r="37" spans="1:4">
+      <c r="A37">
         <v>99998</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B37" t="s">
         <v>649</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C37" t="s">
         <v>650</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D37" t="s">
         <v>650</v>
       </c>
     </row>
@@ -5195,7 +5381,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B2" sqref="B2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8681,10 +8867,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9199,31 +9385,42 @@
         <v>240</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47">
-        <v>99999</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="C47" t="s">
-        <v>272</v>
+    <row r="47" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A47" s="1">
+        <v>58</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
+        <v>99999</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C48" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
         <v>99998</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>650</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -9313,10 +9510,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A2" sqref="A2:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9335,15 +9532,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1">
-      <c r="A2">
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>244</v>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>665</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1">
@@ -9351,10 +9548,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>528</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1">
@@ -9362,10 +9559,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>528</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1">
@@ -9373,114 +9570,158 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1">
       <c r="A6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>247</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>249</v>
-      </c>
-      <c r="C7" t="s">
-        <v>250</v>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1">
       <c r="A8">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C8" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1">
-      <c r="A9">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>253</v>
-      </c>
-      <c r="C9" t="s">
-        <v>254</v>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1">
       <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1">
       <c r="A11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>256</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1">
-      <c r="A12">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
+    <row r="12" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>253</v>
+      </c>
+      <c r="C16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
         <v>99999</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C17" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
+    <row r="18" spans="1:3">
+      <c r="A18">
         <v>99998</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B18" t="s">
         <v>649</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C18" t="s">
         <v>650</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -9493,8 +9734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9713,7 +9954,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Changed 40C, 26F and 720 in UCROffenseCodeType to "Group A"
</commit_message>
<xml_diff>
--- a/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimdouglas/git/nibrs/tools/r-packages/nibrs/inst/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D5C4EC-0597-494E-923F-4206399537A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="1080" windowWidth="20240" windowHeight="12160" tabRatio="705" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="47460" yWindow="3200" windowWidth="20240" windowHeight="12160" tabRatio="705" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -39,7 +45,7 @@
     <sheet name="AgencyType" sheetId="30" r:id="rId30"/>
     <sheet name="CargoTheftIndicatorType" sheetId="31" r:id="rId31"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2082,8 +2088,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2258,13 +2264,16 @@
     <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="TableStyleLight1" xfId="1"/>
+    <cellStyle name="TableStyleLight1" xfId="1" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2556,14 +2565,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -2832,14 +2841,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D33" sqref="D33:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="49.6640625" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
@@ -3375,14 +3384,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
@@ -3510,14 +3519,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="58.1640625" customWidth="1"/>
@@ -4306,14 +4315,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="31.1640625" customWidth="1"/>
     <col min="4" max="4" width="32.33203125" customWidth="1"/>
@@ -4551,14 +4560,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
   </cols>
@@ -4729,14 +4738,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -4874,14 +4883,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="44.6640625" customWidth="1"/>
   </cols>
@@ -5052,14 +5061,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
   </cols>
@@ -5186,14 +5195,14 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" t="s">
@@ -5262,14 +5271,14 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="35.1640625" customWidth="1"/>
   </cols>
@@ -5377,14 +5386,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="26.5" customWidth="1"/>
   </cols>
@@ -5478,14 +5487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" s="4" t="s">
@@ -5554,14 +5563,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" s="4" t="s">
@@ -5630,14 +5639,14 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="46.1640625" customWidth="1"/>
   </cols>
@@ -5874,14 +5883,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="63.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -6008,14 +6017,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
@@ -6153,14 +6162,14 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="40.1640625" customWidth="1"/>
   </cols>
@@ -6488,14 +6497,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
   </cols>
@@ -6578,14 +6587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -6657,14 +6666,14 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="60.1640625" customWidth="1"/>
   </cols>
@@ -6802,14 +6811,14 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
   </cols>
@@ -6881,14 +6890,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -7004,14 +7013,14 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="1"/>
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
@@ -7160,14 +7169,14 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
   </cols>
@@ -7238,14 +7247,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="59.1640625" customWidth="1"/>
@@ -8600,7 +8609,7 @@
         <v>486</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>271</v>
@@ -8623,7 +8632,7 @@
         <v>488</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>271</v>
@@ -8646,7 +8655,7 @@
         <v>481</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>271</v>
@@ -8765,14 +8774,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -8866,14 +8875,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="43.5" customWidth="1"/>
@@ -9430,14 +9439,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
   </cols>
@@ -9509,14 +9518,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="65.5" customWidth="1"/>
   </cols>
@@ -9731,14 +9740,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
   </cols>

</xml_diff>

<commit_message>
Add 90I back to the offense code table.
</commit_message>
<xml_diff>
--- a/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimdouglas/Desktop/Temp/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0D4F68-634C-C847-9856-E885AEEC071A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42640" yWindow="2600" windowWidth="25620" windowHeight="16200" tabRatio="705" firstSheet="26" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="20480" windowHeight="12400" tabRatio="705" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -45,7 +39,7 @@
     <sheet name="AgencyType" sheetId="30" r:id="rId30"/>
     <sheet name="CargoTheftIndicatorType" sheetId="31" r:id="rId31"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -55,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="679">
   <si>
     <t>Table</t>
   </si>
@@ -2086,13 +2080,19 @@
   </si>
   <si>
     <t>Not a Cargo Theft offense</t>
+  </si>
+  <si>
+    <t>90I</t>
+  </si>
+  <si>
+    <t>Runaway</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2145,9 +2145,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="52">
+  <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2217,7 +2219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="52">
+  <cellStyles count="54">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2243,6 +2245,7 @@
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2268,8 +2271,9 @@
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="TableStyleLight1" xfId="1" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2570,14 +2574,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -2846,14 +2850,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="49.6640625" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
@@ -3403,14 +3407,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
@@ -3538,14 +3542,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="58.1640625" customWidth="1"/>
@@ -4334,14 +4338,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="31.1640625" customWidth="1"/>
     <col min="4" max="4" width="32.33203125" customWidth="1"/>
@@ -4579,14 +4583,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
   </cols>
@@ -4757,14 +4761,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -4902,14 +4906,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="44.6640625" customWidth="1"/>
   </cols>
@@ -5080,14 +5084,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
   </cols>
@@ -5214,14 +5218,14 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" t="s">
@@ -5290,14 +5294,14 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="35.1640625" customWidth="1"/>
   </cols>
@@ -5405,14 +5409,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="26.5" customWidth="1"/>
   </cols>
@@ -5495,14 +5499,14 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" s="4" t="s">
@@ -5571,14 +5575,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" s="4" t="s">
@@ -5647,14 +5651,14 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="46.1640625" customWidth="1"/>
   </cols>
@@ -5891,14 +5895,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="63.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -6025,14 +6029,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
@@ -6170,14 +6174,14 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="40.1640625" customWidth="1"/>
   </cols>
@@ -6505,14 +6509,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
   </cols>
@@ -6595,14 +6599,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -6674,14 +6678,14 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="60.1640625" customWidth="1"/>
   </cols>
@@ -6819,14 +6823,14 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
   </cols>
@@ -6898,14 +6902,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -7021,14 +7025,14 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="1"/>
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
@@ -7177,14 +7181,14 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
   </cols>
@@ -7255,14 +7259,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:G29"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="59.1640625" customWidth="1"/>
@@ -8583,15 +8587,15 @@
         <v>506</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" customHeight="1">
-      <c r="A58">
-        <v>910</v>
+    <row r="58" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A58" s="1">
+        <v>909</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C58" t="s">
-        <v>137</v>
+        <v>677</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>678</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>478</v>
@@ -8602,19 +8606,19 @@
       <c r="F58" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="1" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15" customHeight="1">
       <c r="A59">
-        <v>990</v>
+        <v>910</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C59" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>478</v>
@@ -8623,21 +8627,21 @@
         <v>261</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G59" t="s">
-        <v>261</v>
+        <v>506</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15" customHeight="1">
       <c r="A60">
-        <v>701</v>
-      </c>
-      <c r="B60" s="5">
-        <v>720</v>
+        <v>990</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="C60" t="s">
-        <v>471</v>
+        <v>139</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>478</v>
@@ -8646,21 +8650,21 @@
         <v>261</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="G60" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15" customHeight="1">
       <c r="A61">
-        <v>702</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>472</v>
+        <v>701</v>
+      </c>
+      <c r="B61" s="5">
+        <v>720</v>
       </c>
       <c r="C61" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>478</v>
@@ -8669,21 +8673,21 @@
         <v>261</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G61" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62">
-        <v>403</v>
+        <v>702</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="C62" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>478</v>
@@ -8692,44 +8696,44 @@
         <v>261</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G62" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63">
-        <v>641</v>
+        <v>403</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C63" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F63" t="s">
-        <v>500</v>
+      <c r="F63" s="1" t="s">
+        <v>643</v>
       </c>
       <c r="G63" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C64" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>477</v>
@@ -8737,7 +8741,7 @@
       <c r="E64" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" t="s">
         <v>500</v>
       </c>
       <c r="G64" t="s">
@@ -8746,47 +8750,70 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65">
-        <v>99999</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>501</v>
+        <v>642</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>469</v>
       </c>
       <c r="C65" t="s">
-        <v>262</v>
-      </c>
-      <c r="D65" t="s">
-        <v>262</v>
-      </c>
-      <c r="E65" t="s">
-        <v>262</v>
-      </c>
-      <c r="F65" t="s">
-        <v>262</v>
+        <v>470</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>500</v>
       </c>
       <c r="G65" t="s">
-        <v>262</v>
+        <v>503</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66">
+        <v>99999</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="C66" t="s">
+        <v>262</v>
+      </c>
+      <c r="D66" t="s">
+        <v>262</v>
+      </c>
+      <c r="E66" t="s">
+        <v>262</v>
+      </c>
+      <c r="F66" t="s">
+        <v>262</v>
+      </c>
+      <c r="G66" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67">
         <v>99998</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>633</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>633</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E67" t="s">
         <v>633</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F67" t="s">
         <v>633</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G67" t="s">
         <v>633</v>
       </c>
     </row>
@@ -8795,7 +8822,7 @@
     <sortCondition ref="A2:A64"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -8805,14 +8832,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="38.83203125" customWidth="1"/>
   </cols>
@@ -8906,14 +8933,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="43.5" customWidth="1"/>
@@ -9470,14 +9497,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
   </cols>
@@ -9549,14 +9576,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="65.5" customWidth="1"/>
   </cols>
@@ -9771,14 +9798,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
   </cols>

</xml_diff>

<commit_message>
Added weapon type category
</commit_message>
<xml_diff>
--- a/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="23715" yWindow="2655" windowWidth="20475" windowHeight="12255" tabRatio="705" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="23715" yWindow="2655" windowWidth="20475" windowHeight="12255" tabRatio="705" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="1393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="1394">
   <si>
     <t>Table</t>
   </si>
@@ -4229,6 +4229,9 @@
   </si>
   <si>
     <t>Religion</t>
+  </si>
+  <si>
+    <t>TypeOfWeaponForceInvolvedCategory</t>
   </si>
 </sst>
 </file>
@@ -5038,7 +5041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31:D35"/>
     </sheetView>
   </sheetViews>
@@ -16587,8 +16590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -16609,7 +16612,7 @@
         <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>515</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Reverted to previous file.
</commit_message>
<xml_diff>
--- a/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimdouglas/Desktop/Temp/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D04D02B-169F-1E4C-8C1E-83176789CA0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41000" yWindow="1360" windowWidth="24140" windowHeight="14780" tabRatio="705" firstSheet="27" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23715" yWindow="2655" windowWidth="20475" windowHeight="12255" tabRatio="705" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -46,7 +40,7 @@
     <sheet name="CargoTheftIndicatorType" sheetId="31" r:id="rId31"/>
     <sheet name="NibrsErrorCodeType" sheetId="32" r:id="rId32"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -4243,7 +4237,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -4372,7 +4366,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4390,9 +4384,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4462,7 +4453,7 @@
     <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="TableStyleLight1" xfId="1" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4520,7 +4511,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4553,26 +4544,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4605,23 +4579,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4797,16 +4754,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5081,17 +5038,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31:D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="49.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="49.625" customWidth="1"/>
+    <col min="4" max="4" width="31.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
@@ -5638,17 +5595,17 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="8.83203125" style="3"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="3"/>
+    <col min="3" max="3" width="29.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -5773,17 +5730,17 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="8.83203125" style="3"/>
-    <col min="3" max="3" width="58.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="3"/>
+    <col min="3" max="3" width="58.125" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6569,17 +6526,17 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31.125" customWidth="1"/>
+    <col min="4" max="4" width="32.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -6814,16 +6771,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -6992,14 +6949,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -7137,16 +7094,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="3" max="3" width="44.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -7315,14 +7272,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
   </cols>
@@ -7449,14 +7406,14 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" t="s">
@@ -7525,16 +7482,16 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="35.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -7640,14 +7597,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="26.5" customWidth="1"/>
   </cols>
@@ -7730,14 +7687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" s="4" t="s">
@@ -7806,14 +7763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" s="4" t="s">
@@ -7882,16 +7839,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="46.1640625" customWidth="1"/>
+    <col min="3" max="3" width="46.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -8126,14 +8083,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="63.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -8260,14 +8217,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
@@ -8405,16 +8362,16 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="54.83203125" customWidth="1"/>
+    <col min="3" max="3" width="40.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -8740,16 +8697,16 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -8830,14 +8787,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -8909,16 +8866,16 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="60.1640625" customWidth="1"/>
+    <col min="3" max="3" width="60.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -9054,16 +9011,16 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -9133,16 +9090,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -9256,17 +9213,17 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="1"/>
+    <col min="3" max="3" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -9412,18 +9369,16 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -9464,7 +9419,7 @@
         <v>99998</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>630</v>
       </c>
       <c r="C4" t="s">
         <v>674</v>
@@ -9474,7 +9429,7 @@
       <c r="A5">
         <v>99999</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5">
         <v>9</v>
       </c>
       <c r="C5" t="s">
@@ -9492,20 +9447,20 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E267" sqref="E267"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="129.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="2" width="8.875" style="1"/>
+    <col min="3" max="3" width="19.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="129.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -14093,21 +14048,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView topLeftCell="A50" workbookViewId="0">
       <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="8.83203125" style="3"/>
-    <col min="3" max="3" width="59.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="37.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="3"/>
+    <col min="3" max="3" width="59.125" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
+    <col min="5" max="5" width="16.875" customWidth="1"/>
+    <col min="6" max="6" width="37.625" customWidth="1"/>
+    <col min="7" max="7" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
@@ -15666,16 +15621,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="38.83203125" customWidth="1"/>
+    <col min="3" max="3" width="38.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -15767,16 +15722,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="8.83203125" style="3"/>
+    <col min="2" max="2" width="8.875" style="3"/>
     <col min="3" max="3" width="43.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16331,16 +16286,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -16410,14 +16365,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="65.5" customWidth="1"/>
   </cols>
@@ -16632,18 +16587,18 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="8.83203125" style="3"/>
-    <col min="3" max="3" width="26.1640625" customWidth="1"/>
-    <col min="4" max="4" width="35.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="3"/>
+    <col min="3" max="3" width="26.25" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">

</xml_diff>